<commit_message>
Inclusion of link to download of keywords and SwapJD >> MPShufleJD
</commit_message>
<xml_diff>
--- a/analyzes/Execution Results.xlsx
+++ b/analyzes/Execution Results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClaudineiBJr\Documents\Repositories\mt_project\analyzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DFCB04-4F51-41A8-BDA2-75E3666718BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D778E06F-4C66-4963-80BD-C7386AB03BC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{B5B55D40-2CCC-49DC-A42D-814F6A3BB04F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{B5B55D40-2CCC-49DC-A42D-814F6A3BB04F}"/>
   </bookViews>
   <sheets>
     <sheet name="MPTitle" sheetId="1" r:id="rId1"/>
     <sheet name="MPublished" sheetId="2" r:id="rId2"/>
-    <sheet name="SwapJD" sheetId="3" r:id="rId3"/>
+    <sheet name="MPShuffleJD" sheetId="3" r:id="rId3"/>
     <sheet name="Top1Absent" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -32,65 +32,35 @@
     <definedName name="_xlchart.v1.18" hidden="1">MPublished!$F$1</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">MPublished!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">MPTitle!$C$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">MPublished!$B$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">MPublished!$B$2:$B$34</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">MPublished!$C$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">MPublished!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">MPublished!$D$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">MPublished!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">MPublished!$E$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">MPublished!$E$2:$E$34</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">MPublished!$F$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">MPublished!$F$2:$F$34</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">MPShuffleJD!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">MPShuffleJD!$B$2:$B$34</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">MPShuffleJD!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">MPShuffleJD!$C$2:$C$34</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">MPShuffleJD!$D$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">MPShuffleJD!$D$2:$D$34</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">MPShuffleJD!$E$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">MPShuffleJD!$E$2:$E$34</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">MPShuffleJD!$F$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">MPShuffleJD!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">MPTitle!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">SwapJD!$B$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">SwapJD!$B$2:$B$34</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">SwapJD!$C$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">SwapJD!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">SwapJD!$D$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">SwapJD!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">SwapJD!$E$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">SwapJD!$E$2:$E$34</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">SwapJD!$F$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">SwapJD!$F$2:$F$34</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Top1Absent!$B$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Top1Absent!$B$2:$B$34</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Top1Absent!$C$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Top1Absent!$C$2:$C$34</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Top1Absent!$D$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Top1Absent!$D$2:$D$34</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Top1Absent!$E$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Top1Absent!$E$2:$E$34</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Top1Absent!$F$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Top1Absent!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">MPTitle!$D$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Top1Absent!$B$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Top1Absent!$B$2:$B$34</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Top1Absent!$C$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Top1Absent!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Top1Absent!$D$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Top1Absent!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Top1Absent!$E$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Top1Absent!$E$2:$E$34</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Top1Absent!$F$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Top1Absent!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">MPTitle!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Top1Absent!$B$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Top1Absent!$B$2:$B$34</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Top1Absent!$C$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Top1Absent!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Top1Absent!$D$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Top1Absent!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Top1Absent!$E$1</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Top1Absent!$E$2:$E$34</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Top1Absent!$F$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Top1Absent!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">MPTitle!$E$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Top1Absent!$B$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Top1Absent!$B$2:$B$34</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Top1Absent!$C$1</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Top1Absent!$C$2:$C$34</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Top1Absent!$D$1</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Top1Absent!$D$2:$D$34</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Top1Absent!$E$1</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Top1Absent!$E$2:$E$34</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Top1Absent!$F$1</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Top1Absent!$F$2:$F$34</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">MPTitle!$E$2:$E$34</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">MPTitle!$F$1</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">MPTitle!$F$2:$F$34</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2666,27 +2636,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.31</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2696,7 +2666,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7CC7F838-7B36-4F39-B2E8-E8FC70A74AF0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>ACM</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2709,7 +2679,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D6AB601F-D611-4302-956E-2CE4570F974D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.32</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>IEEE v1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2722,7 +2692,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{EEEAACE9-9336-4E63-AA15-0ED8187A02E3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.34</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>IEEE v2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2735,7 +2705,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C25FE34D-CA6F-4F19-B88A-4CC0EC1365B8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.36</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>SciDirect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2748,7 +2718,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E2C118FD-E556-4430-8F6E-85732298DA6C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>Springer</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2831,27 +2801,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.31</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.33</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.45</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.47</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.49</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2861,7 +2831,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3DE7EEF6-92BB-45C1-A7D0-00AE0513A1DD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:f>_xlchart.v1.30</cx:f>
               <cx:v>ACM</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2874,7 +2844,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8CF02960-D0E6-4E2D-85ED-6839C63D86FE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:f>_xlchart.v1.32</cx:f>
               <cx:v>IEEE v1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2887,7 +2857,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{88A3C6E0-8703-49CD-B2BE-83C78547F63F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.44</cx:f>
+              <cx:f>_xlchart.v1.34</cx:f>
               <cx:v>IEEE v2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2900,7 +2870,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{246CD6AE-4491-4D65-90D7-7D0D8AD94804}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.46</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>SciDirect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2913,7 +2883,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9E9F3782-F082-498F-AE6C-C9CB69FFE9D4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
               <cx:v>Springer</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5509,8 +5479,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6174443" y="4022911"/>
-              <a:ext cx="4885764" cy="2991969"/>
+              <a:off x="6207500" y="4019549"/>
+              <a:ext cx="4915460" cy="2991969"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7794,7 +7764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6625FAF6-6B77-40F3-831B-43A5AA87246B}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -8677,7 +8647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E516CF-1252-43BF-A65B-38A1E73C26B5}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>

</xml_diff>